<commit_message>
Aggregates industrial sectors in io data to match indst BIFUbC
</commit_message>
<xml_diff>
--- a/InputData/io-model/BVAbIC/BAU Value Added by ISIC Code.xlsx
+++ b/InputData/io-model/BVAbIC/BAU Value Added by ISIC Code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\io-model\BVAbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F33E950-E379-4B8C-8154-8FF050118181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC3E19C-C89C-49CA-AB98-C843D817DDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2109" uniqueCount="1298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="1300">
   <si>
     <t>Source:</t>
   </si>
@@ -3936,21 +3936,29 @@
   </si>
   <si>
     <t>EU ISIC Groupings</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/databrowser/view/tec00115/default/table?lang=en</t>
+  </si>
+  <si>
+    <t>As the most recent OECD Input-Output Data is available for is 2018, we scale by GDP growth to 2022 from eurostat:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
     <numFmt numFmtId="167" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="#,##0.0;\-#,##0.0;&quot;-&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="172" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4090,6 +4098,13 @@
     <font>
       <sz val="8"/>
       <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4464,12 +4479,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4695,6 +4711,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -4749,30 +4785,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{3ADF3FF5-E4D2-4BC8-9960-7408DCCB591E}"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5087,10 +5107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5260,6 +5280,22 @@
       </c>
       <c r="B38" t="s">
         <v>1215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="104">
+        <f>0.019-0.056+0.063+0.035</f>
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5275,17 +5311,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC40CF3-8B3B-41DC-A935-B8F6C9564C97}">
-  <dimension ref="A1:AU50"/>
+  <dimension ref="A1:AU54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.453125" style="6" customWidth="1"/>
     <col min="2" max="2" width="2.453125" style="6" customWidth="1"/>
-    <col min="3" max="23" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="23" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="24" max="26" width="9.54296875" style="6" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="31" max="36" width="9.54296875" style="6" bestFit="1" customWidth="1"/>
@@ -5314,222 +5351,222 @@
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="104" t="s">
+      <c r="B3" s="106"/>
+      <c r="C3" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
-      <c r="Y3" s="105"/>
-      <c r="Z3" s="105"/>
-      <c r="AA3" s="105"/>
-      <c r="AB3" s="105"/>
-      <c r="AC3" s="105"/>
-      <c r="AD3" s="105"/>
-      <c r="AE3" s="105"/>
-      <c r="AF3" s="105"/>
-      <c r="AG3" s="105"/>
-      <c r="AH3" s="105"/>
-      <c r="AI3" s="105"/>
-      <c r="AJ3" s="105"/>
-      <c r="AK3" s="105"/>
-      <c r="AL3" s="105"/>
-      <c r="AM3" s="105"/>
-      <c r="AN3" s="105"/>
-      <c r="AO3" s="105"/>
-      <c r="AP3" s="105"/>
-      <c r="AQ3" s="105"/>
-      <c r="AR3" s="105"/>
-      <c r="AS3" s="105"/>
-      <c r="AT3" s="105"/>
-      <c r="AU3" s="106"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
+      <c r="R3" s="113"/>
+      <c r="S3" s="113"/>
+      <c r="T3" s="113"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="113"/>
+      <c r="Y3" s="113"/>
+      <c r="Z3" s="113"/>
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113"/>
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="113"/>
+      <c r="AE3" s="113"/>
+      <c r="AF3" s="113"/>
+      <c r="AG3" s="113"/>
+      <c r="AH3" s="113"/>
+      <c r="AI3" s="113"/>
+      <c r="AJ3" s="113"/>
+      <c r="AK3" s="113"/>
+      <c r="AL3" s="113"/>
+      <c r="AM3" s="113"/>
+      <c r="AN3" s="113"/>
+      <c r="AO3" s="113"/>
+      <c r="AP3" s="113"/>
+      <c r="AQ3" s="113"/>
+      <c r="AR3" s="113"/>
+      <c r="AS3" s="113"/>
+      <c r="AT3" s="113"/>
+      <c r="AU3" s="114"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="99" t="s">
+      <c r="B4" s="106"/>
+      <c r="C4" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100"/>
-      <c r="X4" s="100"/>
-      <c r="Y4" s="100"/>
-      <c r="Z4" s="100"/>
-      <c r="AA4" s="100"/>
-      <c r="AB4" s="100"/>
-      <c r="AC4" s="100"/>
-      <c r="AD4" s="100"/>
-      <c r="AE4" s="100"/>
-      <c r="AF4" s="100"/>
-      <c r="AG4" s="100"/>
-      <c r="AH4" s="100"/>
-      <c r="AI4" s="100"/>
-      <c r="AJ4" s="100"/>
-      <c r="AK4" s="100"/>
-      <c r="AL4" s="100"/>
-      <c r="AM4" s="100"/>
-      <c r="AN4" s="100"/>
-      <c r="AO4" s="100"/>
-      <c r="AP4" s="100"/>
-      <c r="AQ4" s="100"/>
-      <c r="AR4" s="100"/>
-      <c r="AS4" s="100"/>
-      <c r="AT4" s="100"/>
-      <c r="AU4" s="101"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="108"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="108"/>
+      <c r="W4" s="108"/>
+      <c r="X4" s="108"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="108"/>
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="108"/>
+      <c r="AD4" s="108"/>
+      <c r="AE4" s="108"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="108"/>
+      <c r="AH4" s="108"/>
+      <c r="AI4" s="108"/>
+      <c r="AJ4" s="108"/>
+      <c r="AK4" s="108"/>
+      <c r="AL4" s="108"/>
+      <c r="AM4" s="108"/>
+      <c r="AN4" s="108"/>
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="108"/>
+      <c r="AQ4" s="108"/>
+      <c r="AR4" s="108"/>
+      <c r="AS4" s="108"/>
+      <c r="AT4" s="108"/>
+      <c r="AU4" s="109"/>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="99" t="s">
+      <c r="B5" s="106"/>
+      <c r="C5" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="100"/>
-      <c r="U5" s="100"/>
-      <c r="V5" s="100"/>
-      <c r="W5" s="100"/>
-      <c r="X5" s="100"/>
-      <c r="Y5" s="100"/>
-      <c r="Z5" s="100"/>
-      <c r="AA5" s="100"/>
-      <c r="AB5" s="100"/>
-      <c r="AC5" s="100"/>
-      <c r="AD5" s="100"/>
-      <c r="AE5" s="100"/>
-      <c r="AF5" s="100"/>
-      <c r="AG5" s="100"/>
-      <c r="AH5" s="100"/>
-      <c r="AI5" s="100"/>
-      <c r="AJ5" s="100"/>
-      <c r="AK5" s="100"/>
-      <c r="AL5" s="100"/>
-      <c r="AM5" s="100"/>
-      <c r="AN5" s="100"/>
-      <c r="AO5" s="100"/>
-      <c r="AP5" s="100"/>
-      <c r="AQ5" s="100"/>
-      <c r="AR5" s="100"/>
-      <c r="AS5" s="100"/>
-      <c r="AT5" s="100"/>
-      <c r="AU5" s="101"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="108"/>
+      <c r="AH5" s="108"/>
+      <c r="AI5" s="108"/>
+      <c r="AJ5" s="108"/>
+      <c r="AK5" s="108"/>
+      <c r="AL5" s="108"/>
+      <c r="AM5" s="108"/>
+      <c r="AN5" s="108"/>
+      <c r="AO5" s="108"/>
+      <c r="AP5" s="108"/>
+      <c r="AQ5" s="108"/>
+      <c r="AR5" s="108"/>
+      <c r="AS5" s="108"/>
+      <c r="AT5" s="108"/>
+      <c r="AU5" s="109"/>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="99" t="s">
+      <c r="B6" s="106"/>
+      <c r="C6" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="100"/>
-      <c r="W6" s="100"/>
-      <c r="X6" s="100"/>
-      <c r="Y6" s="100"/>
-      <c r="Z6" s="100"/>
-      <c r="AA6" s="100"/>
-      <c r="AB6" s="100"/>
-      <c r="AC6" s="100"/>
-      <c r="AD6" s="100"/>
-      <c r="AE6" s="100"/>
-      <c r="AF6" s="100"/>
-      <c r="AG6" s="100"/>
-      <c r="AH6" s="100"/>
-      <c r="AI6" s="100"/>
-      <c r="AJ6" s="100"/>
-      <c r="AK6" s="100"/>
-      <c r="AL6" s="100"/>
-      <c r="AM6" s="100"/>
-      <c r="AN6" s="100"/>
-      <c r="AO6" s="100"/>
-      <c r="AP6" s="100"/>
-      <c r="AQ6" s="100"/>
-      <c r="AR6" s="100"/>
-      <c r="AS6" s="100"/>
-      <c r="AT6" s="100"/>
-      <c r="AU6" s="101"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="108"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="108"/>
+      <c r="T6" s="108"/>
+      <c r="U6" s="108"/>
+      <c r="V6" s="108"/>
+      <c r="W6" s="108"/>
+      <c r="X6" s="108"/>
+      <c r="Y6" s="108"/>
+      <c r="Z6" s="108"/>
+      <c r="AA6" s="108"/>
+      <c r="AB6" s="108"/>
+      <c r="AC6" s="108"/>
+      <c r="AD6" s="108"/>
+      <c r="AE6" s="108"/>
+      <c r="AF6" s="108"/>
+      <c r="AG6" s="108"/>
+      <c r="AH6" s="108"/>
+      <c r="AI6" s="108"/>
+      <c r="AJ6" s="108"/>
+      <c r="AK6" s="108"/>
+      <c r="AL6" s="108"/>
+      <c r="AM6" s="108"/>
+      <c r="AN6" s="108"/>
+      <c r="AO6" s="108"/>
+      <c r="AP6" s="108"/>
+      <c r="AQ6" s="108"/>
+      <c r="AR6" s="108"/>
+      <c r="AS6" s="108"/>
+      <c r="AT6" s="108"/>
+      <c r="AU6" s="109"/>
     </row>
     <row r="7" spans="1:47" ht="110" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="111"/>
       <c r="C7" s="8" t="s">
         <v>46</v>
       </c>
@@ -11675,6 +11712,12 @@
     <row r="50" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="C54" s="123">
+        <f>SUM(C48:AU48)</f>
+        <v>17550249.699999996</v>
       </c>
     </row>
   </sheetData>
@@ -11703,15 +11746,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D6539F-95C5-4167-917F-8B37443DA7CE}">
   <dimension ref="A1:BD1360"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
@@ -11757,186 +11801,186 @@
         <v>42</v>
       </c>
       <c r="B3" s="71"/>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="110"/>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110"/>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="110"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="110"/>
-      <c r="AG3" s="110"/>
-      <c r="AH3" s="110"/>
-      <c r="AI3" s="110"/>
-      <c r="AJ3" s="110"/>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="110"/>
-      <c r="AM3" s="110"/>
-      <c r="AN3" s="110"/>
-      <c r="AO3" s="110"/>
-      <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
-      <c r="AR3" s="110"/>
-      <c r="AS3" s="110"/>
-      <c r="AT3" s="110"/>
-      <c r="AU3" s="110"/>
-      <c r="AV3" s="110"/>
-      <c r="AW3" s="110"/>
-      <c r="AX3" s="110"/>
-      <c r="AY3" s="110"/>
-      <c r="AZ3" s="110"/>
-      <c r="BA3" s="110"/>
-      <c r="BB3" s="110"/>
-      <c r="BC3" s="110"/>
-      <c r="BD3" s="111"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="118"/>
+      <c r="W3" s="118"/>
+      <c r="X3" s="118"/>
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118"/>
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
+      <c r="AG3" s="118"/>
+      <c r="AH3" s="118"/>
+      <c r="AI3" s="118"/>
+      <c r="AJ3" s="118"/>
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="118"/>
+      <c r="AN3" s="118"/>
+      <c r="AO3" s="118"/>
+      <c r="AP3" s="118"/>
+      <c r="AQ3" s="118"/>
+      <c r="AR3" s="118"/>
+      <c r="AS3" s="118"/>
+      <c r="AT3" s="118"/>
+      <c r="AU3" s="118"/>
+      <c r="AV3" s="118"/>
+      <c r="AW3" s="118"/>
+      <c r="AX3" s="118"/>
+      <c r="AY3" s="118"/>
+      <c r="AZ3" s="118"/>
+      <c r="BA3" s="118"/>
+      <c r="BB3" s="118"/>
+      <c r="BC3" s="118"/>
+      <c r="BD3" s="119"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="70" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="71"/>
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="120" t="s">
         <v>1159</v>
       </c>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="113"/>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="113"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="113"/>
-      <c r="W4" s="113"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="113"/>
-      <c r="Z4" s="113"/>
-      <c r="AA4" s="113"/>
-      <c r="AB4" s="113"/>
-      <c r="AC4" s="113"/>
-      <c r="AD4" s="113"/>
-      <c r="AE4" s="113"/>
-      <c r="AF4" s="113"/>
-      <c r="AG4" s="113"/>
-      <c r="AH4" s="113"/>
-      <c r="AI4" s="113"/>
-      <c r="AJ4" s="113"/>
-      <c r="AK4" s="113"/>
-      <c r="AL4" s="113"/>
-      <c r="AM4" s="113"/>
-      <c r="AN4" s="113"/>
-      <c r="AO4" s="113"/>
-      <c r="AP4" s="113"/>
-      <c r="AQ4" s="113"/>
-      <c r="AR4" s="113"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="113"/>
-      <c r="AU4" s="113"/>
-      <c r="AV4" s="113"/>
-      <c r="AW4" s="113"/>
-      <c r="AX4" s="113"/>
-      <c r="AY4" s="113"/>
-      <c r="AZ4" s="113"/>
-      <c r="BA4" s="113"/>
-      <c r="BB4" s="113"/>
-      <c r="BC4" s="113"/>
-      <c r="BD4" s="114"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="121"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="121"/>
+      <c r="T4" s="121"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="121"/>
+      <c r="X4" s="121"/>
+      <c r="Y4" s="121"/>
+      <c r="Z4" s="121"/>
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="121"/>
+      <c r="AC4" s="121"/>
+      <c r="AD4" s="121"/>
+      <c r="AE4" s="121"/>
+      <c r="AF4" s="121"/>
+      <c r="AG4" s="121"/>
+      <c r="AH4" s="121"/>
+      <c r="AI4" s="121"/>
+      <c r="AJ4" s="121"/>
+      <c r="AK4" s="121"/>
+      <c r="AL4" s="121"/>
+      <c r="AM4" s="121"/>
+      <c r="AN4" s="121"/>
+      <c r="AO4" s="121"/>
+      <c r="AP4" s="121"/>
+      <c r="AQ4" s="121"/>
+      <c r="AR4" s="121"/>
+      <c r="AS4" s="121"/>
+      <c r="AT4" s="121"/>
+      <c r="AU4" s="121"/>
+      <c r="AV4" s="121"/>
+      <c r="AW4" s="121"/>
+      <c r="AX4" s="121"/>
+      <c r="AY4" s="121"/>
+      <c r="AZ4" s="121"/>
+      <c r="BA4" s="121"/>
+      <c r="BB4" s="121"/>
+      <c r="BC4" s="121"/>
+      <c r="BD4" s="122"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A5" s="70" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="71"/>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="113"/>
-      <c r="N5" s="113"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="113"/>
-      <c r="T5" s="113"/>
-      <c r="U5" s="113"/>
-      <c r="V5" s="113"/>
-      <c r="W5" s="113"/>
-      <c r="X5" s="113"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="113"/>
-      <c r="AH5" s="113"/>
-      <c r="AI5" s="113"/>
-      <c r="AJ5" s="113"/>
-      <c r="AK5" s="113"/>
-      <c r="AL5" s="113"/>
-      <c r="AM5" s="113"/>
-      <c r="AN5" s="113"/>
-      <c r="AO5" s="113"/>
-      <c r="AP5" s="113"/>
-      <c r="AQ5" s="113"/>
-      <c r="AR5" s="113"/>
-      <c r="AS5" s="113"/>
-      <c r="AT5" s="113"/>
-      <c r="AU5" s="113"/>
-      <c r="AV5" s="113"/>
-      <c r="AW5" s="113"/>
-      <c r="AX5" s="113"/>
-      <c r="AY5" s="113"/>
-      <c r="AZ5" s="113"/>
-      <c r="BA5" s="113"/>
-      <c r="BB5" s="113"/>
-      <c r="BC5" s="113"/>
-      <c r="BD5" s="114"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="121"/>
+      <c r="T5" s="121"/>
+      <c r="U5" s="121"/>
+      <c r="V5" s="121"/>
+      <c r="W5" s="121"/>
+      <c r="X5" s="121"/>
+      <c r="Y5" s="121"/>
+      <c r="Z5" s="121"/>
+      <c r="AA5" s="121"/>
+      <c r="AB5" s="121"/>
+      <c r="AC5" s="121"/>
+      <c r="AD5" s="121"/>
+      <c r="AE5" s="121"/>
+      <c r="AF5" s="121"/>
+      <c r="AG5" s="121"/>
+      <c r="AH5" s="121"/>
+      <c r="AI5" s="121"/>
+      <c r="AJ5" s="121"/>
+      <c r="AK5" s="121"/>
+      <c r="AL5" s="121"/>
+      <c r="AM5" s="121"/>
+      <c r="AN5" s="121"/>
+      <c r="AO5" s="121"/>
+      <c r="AP5" s="121"/>
+      <c r="AQ5" s="121"/>
+      <c r="AR5" s="121"/>
+      <c r="AS5" s="121"/>
+      <c r="AT5" s="121"/>
+      <c r="AU5" s="121"/>
+      <c r="AV5" s="121"/>
+      <c r="AW5" s="121"/>
+      <c r="AX5" s="121"/>
+      <c r="AY5" s="121"/>
+      <c r="AZ5" s="121"/>
+      <c r="BA5" s="121"/>
+      <c r="BB5" s="121"/>
+      <c r="BC5" s="121"/>
+      <c r="BD5" s="122"/>
     </row>
     <row r="6" spans="1:56" ht="160" x14ac:dyDescent="0.35">
       <c r="A6" s="68" t="s">
@@ -12277,7 +12321,7 @@
       </c>
     </row>
     <row r="8" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="115" t="s">
         <v>131</v>
       </c>
       <c r="B8" s="63" t="s">
@@ -12447,7 +12491,7 @@
       </c>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A9" s="108"/>
+      <c r="A9" s="116"/>
       <c r="B9" s="63" t="s">
         <v>1188</v>
       </c>
@@ -12615,7 +12659,7 @@
       </c>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A10" s="108"/>
+      <c r="A10" s="116"/>
       <c r="B10" s="63" t="s">
         <v>1189</v>
       </c>
@@ -12783,7 +12827,7 @@
       </c>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A11" s="108"/>
+      <c r="A11" s="116"/>
       <c r="B11" s="63" t="s">
         <v>1190</v>
       </c>
@@ -12951,7 +12995,7 @@
       </c>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A12" s="108"/>
+      <c r="A12" s="116"/>
       <c r="B12" s="63" t="s">
         <v>1191</v>
       </c>
@@ -13119,7 +13163,7 @@
       </c>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A13" s="108"/>
+      <c r="A13" s="116"/>
       <c r="B13" s="63" t="s">
         <v>1192</v>
       </c>
@@ -13287,7 +13331,7 @@
       </c>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A14" s="108"/>
+      <c r="A14" s="116"/>
       <c r="B14" s="63" t="s">
         <v>1193</v>
       </c>
@@ -13455,7 +13499,7 @@
       </c>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A15" s="108"/>
+      <c r="A15" s="116"/>
       <c r="B15" s="63" t="s">
         <v>1194</v>
       </c>
@@ -13623,7 +13667,7 @@
       </c>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A16" s="108"/>
+      <c r="A16" s="116"/>
       <c r="B16" s="63" t="s">
         <v>1195</v>
       </c>
@@ -13791,7 +13835,7 @@
       </c>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A17" s="108"/>
+      <c r="A17" s="116"/>
       <c r="B17" s="63" t="s">
         <v>1196</v>
       </c>
@@ -13959,7 +14003,7 @@
       </c>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A18" s="108"/>
+      <c r="A18" s="116"/>
       <c r="B18" s="63" t="s">
         <v>1197</v>
       </c>
@@ -14127,7 +14171,7 @@
       </c>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A19" s="108"/>
+      <c r="A19" s="116"/>
       <c r="B19" s="63" t="s">
         <v>1198</v>
       </c>
@@ -14295,7 +14339,7 @@
       </c>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A20" s="108"/>
+      <c r="A20" s="116"/>
       <c r="B20" s="63" t="s">
         <v>1199</v>
       </c>
@@ -14463,7 +14507,7 @@
       </c>
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A21" s="108"/>
+      <c r="A21" s="116"/>
       <c r="B21" s="63" t="s">
         <v>1200</v>
       </c>
@@ -14631,7 +14675,7 @@
       </c>
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A22" s="108"/>
+      <c r="A22" s="116"/>
       <c r="B22" s="63" t="s">
         <v>1201</v>
       </c>
@@ -14799,7 +14843,7 @@
       </c>
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A23" s="108"/>
+      <c r="A23" s="116"/>
       <c r="B23" s="63" t="s">
         <v>1202</v>
       </c>
@@ -14967,7 +15011,7 @@
       </c>
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A24" s="108"/>
+      <c r="A24" s="116"/>
       <c r="B24" s="63" t="s">
         <v>1203</v>
       </c>
@@ -15135,7 +15179,7 @@
       </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A25" s="108"/>
+      <c r="A25" s="116"/>
       <c r="B25" s="63" t="s">
         <v>1204</v>
       </c>
@@ -15303,7 +15347,7 @@
       </c>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A26" s="108"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="63" t="s">
         <v>1205</v>
       </c>
@@ -15471,7 +15515,7 @@
       </c>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A27" s="108"/>
+      <c r="A27" s="116"/>
       <c r="B27" s="63" t="s">
         <v>1206</v>
       </c>
@@ -15639,7 +15683,7 @@
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A28" s="108"/>
+      <c r="A28" s="116"/>
       <c r="B28" s="63" t="s">
         <v>1207</v>
       </c>
@@ -15807,7 +15851,7 @@
       </c>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A29" s="108"/>
+      <c r="A29" s="116"/>
       <c r="B29" s="63" t="s">
         <v>1208</v>
       </c>
@@ -15975,7 +16019,7 @@
       </c>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A30" s="108"/>
+      <c r="A30" s="116"/>
       <c r="B30" s="63" t="s">
         <v>1209</v>
       </c>
@@ -16143,7 +16187,7 @@
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A31" s="108"/>
+      <c r="A31" s="116"/>
       <c r="B31" s="63" t="s">
         <v>1210</v>
       </c>
@@ -16311,7 +16355,7 @@
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A32" s="108"/>
+      <c r="A32" s="116"/>
       <c r="B32" s="66" t="s">
         <v>1211</v>
       </c>
@@ -16479,7 +16523,7 @@
       </c>
     </row>
     <row r="33" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A33" s="108"/>
+      <c r="A33" s="116"/>
       <c r="B33" s="63" t="s">
         <v>1212</v>
       </c>
@@ -16647,7 +16691,7 @@
       </c>
     </row>
     <row r="34" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A34" s="108"/>
+      <c r="A34" s="116"/>
       <c r="B34" s="63" t="s">
         <v>1213</v>
       </c>
@@ -17040,6 +17084,17 @@
       <c r="A36" s="67" t="s">
         <v>1214</v>
       </c>
+      <c r="C36" s="124">
+        <f>SUM(C35:BD35)</f>
+        <v>14282712.899999997</v>
+      </c>
+      <c r="D36" s="124">
+        <f>SUM(C35:BD35)*About!A38*(1+About!A42)</f>
+        <v>13850717.965626596</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="C37" s="124"/>
     </row>
     <row r="49" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -18379,7 +18434,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25385,7 +25440,7 @@
   <dimension ref="A1:Z123"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30422,7 +30477,7 @@
   <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30512,10 +30567,10 @@
       <c r="Z1" s="50" t="s">
         <v>1151</v>
       </c>
-      <c r="AA1" s="54" t="s">
+      <c r="AA1" s="51" t="s">
         <v>1152</v>
       </c>
-      <c r="AB1" s="51" t="s">
+      <c r="AB1" s="4" t="s">
         <v>1153</v>
       </c>
       <c r="AC1" s="4" t="s">
@@ -30569,220 +30624,220 @@
         <v>1216</v>
       </c>
       <c r="B2">
-        <f>'OECD TTL EU'!C35*10^6*About!$A$38</f>
-        <v>227783515399.99994</v>
+        <f>SUM('OECD TTL EU'!C35:D35)*10^6*About!$A$38</f>
+        <v>234547663799.99994</v>
       </c>
       <c r="C2" s="52">
-        <f>'OECD TTL'!D48*10^6*About!$A$36*('EU Data for ISIC Splits'!D9/SUM('EU Data for ISIC Splits'!D9:E9))</f>
-        <v>34686962250.554153</v>
+        <f>'OECD TTL'!E48*10^6*About!$A$36*('EU Data for ISIC Splits'!D9/SUM('EU Data for ISIC Splits'!D9:E9))</f>
+        <v>6363773944.9871864</v>
       </c>
       <c r="D2" s="53">
-        <f>'OECD TTL'!D48*10^6*About!$A$36*('EU Data for ISIC Splits'!E9/SUM('EU Data for ISIC Splits'!D9:E9))</f>
-        <v>182741172158.37012</v>
+        <f>'OECD TTL'!E48*10^6*About!$A$36*('EU Data for ISIC Splits'!E9/SUM('EU Data for ISIC Splits'!D9:E9))</f>
+        <v>33526242559.314201</v>
       </c>
       <c r="E2">
-        <f>'OECD TTL EU'!E35*10^6*About!$A$38</f>
-        <v>24271361400</v>
-      </c>
-      <c r="F2">
         <f>'OECD TTL EU'!F35*10^6*About!$A$38</f>
         <v>18934332600</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <f>'OECD TTL EU'!G35*10^6*About!$A$38</f>
         <v>3694570800</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <f>'OECD TTL EU'!H35*10^6*About!$A$38</f>
         <v>262184281800.00006</v>
       </c>
-      <c r="I2">
+      <c r="H2">
         <f>'OECD TTL EU'!I35*10^6*About!$A$38</f>
         <v>73533310800.000015</v>
       </c>
-      <c r="J2">
+      <c r="I2">
         <f>'OECD TTL EU'!J35*10^6*About!$A$38</f>
         <v>39516058800</v>
       </c>
-      <c r="K2">
+      <c r="J2">
         <f>'OECD TTL EU'!K35*10^6*About!$A$38</f>
         <v>79851792800.000031</v>
       </c>
+      <c r="K2">
+        <f>'OECD TTL EU'!L35*10^6*About!$A$38</f>
+        <v>43406865399.999992</v>
+      </c>
       <c r="L2" s="52">
-        <f>'OECD TTL'!L48*10^6*About!$A$36*('EU Data for ISIC Splits'!G9/SUM('EU Data for ISIC Splits'!G9:H9))</f>
-        <v>239208645625.53159</v>
-      </c>
-      <c r="M2" s="53">
-        <f>'OECD TTL'!L48*10^6*About!$A$36*('EU Data for ISIC Splits'!H9/SUM('EU Data for ISIC Splits'!G9:H9))</f>
-        <v>125000513774.84894</v>
+        <f>'OECD TTL'!M48*10^6*About!$A$36</f>
+        <v>77354066881.278564</v>
+      </c>
+      <c r="M2" s="52">
+        <f>'OECD TTL'!N48*10^6*About!$A$36</f>
+        <v>49795366780.44191</v>
       </c>
       <c r="N2">
-        <f>'OECD TTL EU'!M35*10^6*About!$A$38</f>
-        <v>155907378000</v>
+        <f>'OECD TTL EU'!O35*10^6*About!$A$38</f>
+        <v>99438264399.999985</v>
       </c>
       <c r="O2" s="52">
-        <f>'OECD TTL'!N48*10^6*About!$A$36*('EU Data for ISIC Splits'!J9/SUM('EU Data for ISIC Splits'!J9:K9))</f>
-        <v>11551466603.723259</v>
+        <f>'OECD TTL'!P48*10^6*About!$A$36*('EU Data for ISIC Splits'!J9/SUM('EU Data for ISIC Splits'!J9:K9))</f>
+        <v>32983677160.936783</v>
       </c>
       <c r="P2" s="53">
-        <f>'OECD TTL'!N48*10^6*About!$A$36*('EU Data for ISIC Splits'!K9/SUM('EU Data for ISIC Splits'!J9:K9))</f>
-        <v>38243900176.718651</v>
+        <f>'OECD TTL'!P48*10^6*About!$A$36*('EU Data for ISIC Splits'!K9/SUM('EU Data for ISIC Splits'!J9:K9))</f>
+        <v>109200372565.45415</v>
       </c>
       <c r="Q2" s="52">
-        <f>'OECD TTL'!O48*10^6*About!$A$36*('EU Data for ISIC Splits'!M9/SUM('EU Data for ISIC Splits'!M9:N9))</f>
-        <v>34190499295.582779</v>
+        <f>'OECD TTL'!Q48*10^6*About!$A$36*('EU Data for ISIC Splits'!M9/SUM('EU Data for ISIC Splits'!M9:N9))</f>
+        <v>171135299199.20331</v>
       </c>
       <c r="R2" s="53">
-        <f>'OECD TTL'!O48*10^6*About!$A$36*('EU Data for ISIC Splits'!N9/SUM('EU Data for ISIC Splits'!M9:N9))</f>
-        <v>19709752511.671555</v>
+        <f>'OECD TTL'!Q48*10^6*About!$A$36*('EU Data for ISIC Splits'!N9/SUM('EU Data for ISIC Splits'!M9:N9))</f>
+        <v>98654142604.549149</v>
       </c>
       <c r="S2">
-        <f>'OECD TTL EU'!P35*10^6*About!$A$38</f>
-        <v>75187011000.000015</v>
-      </c>
-      <c r="T2">
-        <f>'OECD TTL EU'!Q35*10^6*About!$A$38</f>
-        <v>78857360799.999969</v>
-      </c>
-      <c r="U2">
         <f>'OECD TTL EU'!R35*10^6*About!$A$38</f>
         <v>197125030600</v>
       </c>
-      <c r="V2">
+      <c r="T2">
         <f>'OECD TTL EU'!S35*10^6*About!$A$38</f>
         <v>115193248000.00002</v>
       </c>
-      <c r="W2">
+      <c r="U2">
         <f>'OECD TTL EU'!T35*10^6*About!$A$38</f>
         <v>106210730199.99998</v>
       </c>
-      <c r="X2">
+      <c r="V2">
         <f>'OECD TTL EU'!U35*10^6*About!$A$38</f>
         <v>249868588799.99994</v>
       </c>
-      <c r="Y2">
+      <c r="W2">
         <f>'OECD TTL EU'!V35*10^6*About!$A$38</f>
         <v>252920069200</v>
       </c>
-      <c r="Z2" s="52">
-        <f>'OECD TTL'!W48*10^6*About!$A$36*('EU Data for ISIC Splits'!P9/SUM('EU Data for ISIC Splits'!P9:R9))</f>
-        <v>178253977137.72968</v>
-      </c>
-      <c r="AA2" s="55">
-        <f>'OECD TTL'!W48*10^6*About!$A$36*('EU Data for ISIC Splits'!Q9/SUM('EU Data for ISIC Splits'!P9:R9))</f>
-        <v>50825260799.961174</v>
-      </c>
-      <c r="AB2" s="53">
-        <f>'OECD TTL'!W48*10^6*About!$A$36*('EU Data for ISIC Splits'!R9/SUM('EU Data for ISIC Splits'!P9:R9))</f>
-        <v>67086531240.891289</v>
-      </c>
-      <c r="AC2">
+      <c r="X2">
+        <f>'OECD TTL EU'!W35*10^6*About!$A$38</f>
+        <v>58290349999.999985</v>
+      </c>
+      <c r="Y2">
         <f>'OECD TTL EU'!X35*10^6*About!$A$38</f>
         <v>187767590000</v>
       </c>
-      <c r="AD2">
-        <f>'OECD TTL EU'!Y35*10^6*About!$A$38</f>
-        <v>241587474600.00003</v>
-      </c>
-      <c r="AE2">
-        <f>'OECD TTL EU'!Z35*10^6*About!$A$38</f>
-        <v>124678100199.99994</v>
-      </c>
-      <c r="AF2">
+      <c r="Z2" s="52">
+        <f>'OECD TTL'!Y48*10^6*About!$A$36*('EU Data for ISIC Splits'!P9/SUM('EU Data for ISIC Splits'!P9:Q9))</f>
+        <v>1390559103832.0786</v>
+      </c>
+      <c r="AA2" s="53">
+        <f>'OECD TTL'!Y48*10^6*About!$A$36*('EU Data for ISIC Splits'!Q9/SUM('EU Data for ISIC Splits'!P9:Q9))</f>
+        <v>396487810509.93066</v>
+      </c>
+      <c r="AB2" s="20">
+        <f>'OECD TTL'!Z48*10^6</f>
+        <v>578089200000</v>
+      </c>
+      <c r="AC2">
         <f>'OECD TTL EU'!AA35*10^6*About!$A$38</f>
         <v>692275664800</v>
       </c>
-      <c r="AG2">
+      <c r="AD2">
         <f>'OECD TTL EU'!AB35*10^6*About!$A$38</f>
         <v>1487803441800.0002</v>
       </c>
-      <c r="AH2">
-        <f>'OECD TTL EU'!AC35*10^6*About!$A$38</f>
-        <v>298351627399.99994</v>
-      </c>
-      <c r="AI2">
-        <f>'OECD TTL EU'!AD35*10^6*About!$A$38</f>
-        <v>31068779400</v>
-      </c>
-      <c r="AJ2">
-        <f>'OECD TTL EU'!AE35*10^6*About!$A$38</f>
-        <v>35770852399.999985</v>
-      </c>
-      <c r="AK2">
-        <f>'OECD TTL EU'!AF35*10^6*About!$A$38</f>
-        <v>233078317399.99994</v>
-      </c>
-      <c r="AL2">
-        <f>'OECD TTL EU'!AG35*10^6*About!$A$38</f>
-        <v>49426560800</v>
-      </c>
-      <c r="AM2">
+      <c r="AE2">
+        <f>SUM('OECD TTL EU'!AC35:AG35)*10^6*About!$A$38</f>
+        <v>647696137399.99976</v>
+      </c>
+      <c r="AF2">
         <f>'OECD TTL EU'!AH35*10^6*About!$A$38</f>
         <v>379958848600</v>
       </c>
-      <c r="AN2">
+      <c r="AG2">
         <f>'OECD TTL EU'!AI35*10^6*About!$A$38</f>
         <v>143313097799.99997</v>
       </c>
-      <c r="AO2">
+      <c r="AH2">
         <f>'OECD TTL EU'!AJ35*10^6*About!$A$38</f>
         <v>147048981400</v>
       </c>
-      <c r="AP2">
+      <c r="AI2">
         <f>'OECD TTL EU'!AK35*10^6*About!$A$38</f>
         <v>351052227599.99988</v>
       </c>
-      <c r="AQ2">
+      <c r="AJ2">
         <f>'OECD TTL EU'!AL35*10^6*About!$A$38</f>
         <v>584864669800</v>
       </c>
+      <c r="AK2">
+        <f>'OECD TTL EU'!AM35*10^6*About!$A$38</f>
+        <v>1411654811399.9995</v>
+      </c>
+      <c r="AL2">
+        <f>SUM('OECD TTL EU'!AN35:AO35)*10^6*About!$A$38</f>
+        <v>1472777647400</v>
+      </c>
+      <c r="AM2">
+        <f>'OECD TTL EU'!AP35*10^6*About!$A$38</f>
+        <v>843747583599.99988</v>
+      </c>
+      <c r="AN2">
+        <f>'OECD TTL EU'!AQ35*10^6*About!$A$38</f>
+        <v>634371205600</v>
+      </c>
+      <c r="AO2">
+        <f>'OECD TTL EU'!AR35*10^6*About!$A$38</f>
+        <v>961929246000</v>
+      </c>
+      <c r="AP2">
+        <f>SUM('OECD TTL EU'!AS35:AT35)*10^6*About!$A$38</f>
+        <v>387281633800.00006</v>
+      </c>
+      <c r="AQ2">
+        <f>'OECD TTL EU'!AU35*10^6*About!$A$38</f>
+        <v>49328123000.000008</v>
+      </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="97" t="s">
         <v>1295</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="115"/>
-      <c r="S4" s="115"/>
-      <c r="T4" s="115"/>
-      <c r="U4" s="115"/>
-      <c r="V4" s="115"/>
-      <c r="W4" s="115"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="115"/>
-      <c r="Z4" s="115"/>
-      <c r="AA4" s="115"/>
-      <c r="AB4" s="115"/>
-      <c r="AC4" s="115"/>
-      <c r="AD4" s="115"/>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="115"/>
-      <c r="AG4" s="115"/>
-      <c r="AH4" s="115"/>
-      <c r="AI4" s="115"/>
-      <c r="AJ4" s="115"/>
-      <c r="AK4" s="115"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="115"/>
-      <c r="AN4" s="115"/>
-      <c r="AO4" s="115"/>
-      <c r="AP4" s="115"/>
-      <c r="AQ4" s="115"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="97"/>
+      <c r="Z4" s="97"/>
+      <c r="AA4" s="97"/>
+      <c r="AB4" s="97"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="97"/>
+      <c r="AE4" s="97"/>
+      <c r="AF4" s="97"/>
+      <c r="AG4" s="97"/>
+      <c r="AH4" s="97"/>
+      <c r="AI4" s="97"/>
+      <c r="AJ4" s="97"/>
+      <c r="AK4" s="97"/>
+      <c r="AL4" s="97"/>
+      <c r="AM4" s="97"/>
+      <c r="AN4" s="97"/>
+      <c r="AO4" s="97"/>
+      <c r="AP4" s="97"/>
+      <c r="AQ4" s="97"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -30928,7 +30983,7 @@
       <c r="D6" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="116" t="s">
+      <c r="E6" s="98" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -30955,7 +31010,7 @@
       <c r="M6" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N6" s="116" t="s">
+      <c r="N6" s="98" t="s">
         <v>25</v>
       </c>
       <c r="O6" s="4" t="s">
@@ -30970,25 +31025,25 @@
       <c r="R6" s="4" t="s">
         <v>1150</v>
       </c>
-      <c r="S6" s="117" t="s">
+      <c r="S6" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="117" t="s">
+      <c r="T6" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="117" t="s">
+      <c r="U6" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="V6" s="118" t="s">
+      <c r="V6" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="119" t="s">
+      <c r="W6" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="120" t="s">
+      <c r="X6" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="Y6" s="121" t="s">
+      <c r="Y6" s="103" t="s">
         <v>25</v>
       </c>
       <c r="Z6" s="4" t="s">
@@ -31000,7 +31055,7 @@
       <c r="AB6" s="4" t="s">
         <v>1153</v>
       </c>
-      <c r="AC6" s="116" t="s">
+      <c r="AC6" s="98" t="s">
         <v>25</v>
       </c>
       <c r="AD6" s="4" t="s">
@@ -31059,8 +31114,8 @@
   </sheetPr>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31207,172 +31262,172 @@
         <v>1216</v>
       </c>
       <c r="B2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,B1)</f>
-        <v>227783515399.99994</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,B1)*(1+About!$A42)</f>
+        <v>248855071291.79993</v>
       </c>
       <c r="C2" s="52">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,C1)</f>
-        <v>34686962250.554153</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,C1)*(1+About!$A42)</f>
+        <v>6751964155.6314049</v>
       </c>
       <c r="D2" s="53">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,D1)</f>
-        <v>182741172158.37012</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,D1)*(1+About!$A42)</f>
+        <v>35571343355.432365</v>
       </c>
       <c r="E2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,E1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,E1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,F1)</f>
-        <v>18934332600</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,F1)*(1+About!$A42)</f>
+        <v>3919939618.7999997</v>
       </c>
       <c r="G2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,G1)</f>
-        <v>3694570800</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,G1)*(1+About!$A42)</f>
+        <v>278177522989.80005</v>
       </c>
       <c r="H2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,H1)</f>
-        <v>262184281800.00006</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,H1)*(1+About!$A42)</f>
+        <v>78018842758.800018</v>
       </c>
       <c r="I2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,I1)</f>
-        <v>73533310800.000015</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,I1)*(1+About!$A42)</f>
+        <v>41926538386.799995</v>
       </c>
       <c r="J2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,J1)</f>
-        <v>39516058800</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,J1)*(1+About!$A42)</f>
+        <v>84722752160.800034</v>
       </c>
       <c r="K2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,K1)</f>
-        <v>79851792800.000031</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,K1)*(1+About!$A42)</f>
+        <v>46054684189.399986</v>
       </c>
       <c r="L2" s="52">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,L1)</f>
-        <v>239208645625.53159</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,L1)*(1+About!$A42)</f>
+        <v>82072664961.03656</v>
       </c>
       <c r="M2" s="53">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,M1)</f>
-        <v>125000513774.84894</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,M1)*(1+About!$A42)</f>
+        <v>52832884154.048866</v>
       </c>
       <c r="N2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,N1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,N1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="O2" s="52">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,O1)</f>
-        <v>11551466603.723259</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,O1)*(1+About!$A42)</f>
+        <v>34995681467.753922</v>
       </c>
       <c r="P2" s="53">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,P1)</f>
-        <v>38243900176.718651</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,P1)*(1+About!$A42)</f>
+        <v>115861595291.94684</v>
       </c>
       <c r="Q2" s="52">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,Q1)</f>
-        <v>34190499295.582779</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,Q1)*(1+About!$A42)</f>
+        <v>181574552450.35471</v>
       </c>
       <c r="R2" s="53">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,R1)</f>
-        <v>19709752511.671555</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,R1)*(1+About!$A42)</f>
+        <v>104672045303.42664</v>
       </c>
       <c r="S2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,S1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,S1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,T1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,T1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="U2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,U1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,U1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,V1)</f>
-        <v>466362650400</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,V1)*(1+About!$A42)</f>
+        <v>709169851053.59998</v>
       </c>
       <c r="W2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,W1)</f>
-        <v>356079318999.99994</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,W1)*(1+About!$A42)</f>
+        <v>330194254771.20001</v>
       </c>
       <c r="X2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,X1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,X1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,Y1)</f>
-        <v>620866398600</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,Y1)*(1+About!$A42)</f>
+        <v>1059319218759.7999</v>
       </c>
       <c r="Z2" s="52">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,Z1)</f>
-        <v>178253977137.72968</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,Z1)*(1+About!$A42)</f>
+        <v>1475383209165.8354</v>
       </c>
       <c r="AA2" s="55">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AA1)</f>
-        <v>50825260799.961174</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AA1)*(1+About!$A42)</f>
+        <v>420673566951.03644</v>
       </c>
       <c r="AB2" s="53">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AB1)</f>
-        <v>67086531240.891289</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AB1)*(1+About!$A42)</f>
+        <v>613352641200</v>
       </c>
       <c r="AC2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AC1)</f>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AC1)*(1+About!$A42)</f>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AD1)</f>
-        <v>241587474600.00003</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AD1)*(1+About!$A42)</f>
+        <v>1578559451749.8003</v>
       </c>
       <c r="AE2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AE1)</f>
-        <v>124678100199.99994</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AE1)*(1+About!$A42)</f>
+        <v>687205601781.39966</v>
       </c>
       <c r="AF2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AF1)</f>
-        <v>692275664800</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AF1)*(1+About!$A42)</f>
+        <v>403136338364.59998</v>
       </c>
       <c r="AG2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AG1)</f>
-        <v>1487803441800.0002</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AG1)*(1+About!$A42)</f>
+        <v>152055196765.79996</v>
       </c>
       <c r="AH2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AH1)</f>
-        <v>298351627399.99994</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AH1)*(1+About!$A42)</f>
+        <v>156018969265.39999</v>
       </c>
       <c r="AI2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AI1)</f>
-        <v>31068779400</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AI1)*(1+About!$A42)</f>
+        <v>372466413483.59985</v>
       </c>
       <c r="AJ2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AJ1)</f>
-        <v>35770852399.999985</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AJ1)*(1+About!$A42)</f>
+        <v>620541414657.79993</v>
       </c>
       <c r="AK2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AK1)</f>
-        <v>233078317399.99994</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AK1)*(1+About!$A42)</f>
+        <v>1497765754895.3994</v>
       </c>
       <c r="AL2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AL1)</f>
-        <v>49426560800</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AL1)*(1+About!$A42)</f>
+        <v>1562617083891.3999</v>
       </c>
       <c r="AM2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AM1)</f>
-        <v>379958848600</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AM1)*(1+About!$A42)</f>
+        <v>895216186199.59985</v>
       </c>
       <c r="AN2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AN1)</f>
-        <v>143313097799.99997</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AN1)*(1+About!$A42)</f>
+        <v>673067849141.59998</v>
       </c>
       <c r="AO2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AO1)</f>
-        <v>147048981400</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AO1)*(1+About!$A42)</f>
+        <v>1020606930006</v>
       </c>
       <c r="AP2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AP1)</f>
-        <v>351052227599.99988</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AP1)*(1+About!$A42)</f>
+        <v>410905813461.80005</v>
       </c>
       <c r="AQ2">
-        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AQ1)</f>
-        <v>584864669800</v>
+        <f>SUMIFS('Pre ISIC Consolidation'!$B$2:$AQ$2,'Pre ISIC Consolidation'!$B$6:$AQ$6,AQ1)*(1+About!$A42)</f>
+        <v>52337138503.000008</v>
       </c>
     </row>
   </sheetData>
@@ -31391,6 +31446,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -31613,17 +31679,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F11C581-B9CA-407F-AC4D-3EE1CBBD99D2}">
   <ds:schemaRefs>
@@ -31633,6 +31688,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61760655-2A9D-48D5-B2C9-70E011B3A955}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{348DE86D-E474-4780-86DA-9FDF1AF80B25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31649,15 +31715,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61760655-2A9D-48D5-B2C9-70E011B3A955}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>